<commit_message>
Updated Ck parameter experiment - Added ck dataset - Added script 'run_experiment_training_2016_2017_test_2018_2019.m' to run the ck experiment using the old model dataset configuration
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Ck_Parameters_Estimation/0-Dataset/CK_OBS_WITH_FEATURES.xlsx
+++ b/Parameters-Estimation/Ck_Parameters_Estimation/0-Dataset/CK_OBS_WITH_FEATURES.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\4_Estuarine Box Model\Experiments\Parameters-Estimation\Ck_Parameters_Estimation\0-Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\3_Estuarine Box Model\Experiments\Parameters-Estimation\Ck_Parameters_Estimation\0-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928FFAE1-7173-43D0-8DE6-6D19D0B72ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3ECBA2F-F918-4B7F-9F2F-D7725B544921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ck_Old_Model" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -414,7 +414,7 @@
   <dimension ref="A1:F1643"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -422,7 +422,7 @@
     <col min="1" max="1" width="12.42578125" style="5"/>
     <col min="2" max="2" width="16" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125"/>
-    <col min="4" max="4" width="13" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Updated experiment structure - Updated script to run experiment with training and test set splitted randomly on salinity and ck - Updated 'function remove_missing_data_features.m' - Added function 'plot_boxplot_training_test.m' - Added function 'plot_importance.m' - Deleted old salinity and ck experiment with randomly splitting of dataset
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Ck_Parameters_Estimation/0-Dataset/CK_OBS_WITH_FEATURES.xlsx
+++ b/Parameters-Estimation/Ck_Parameters_Estimation/0-Dataset/CK_OBS_WITH_FEATURES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\3_Estuarine Box Model\Experiments\Parameters-Estimation\Ck_Parameters_Estimation\0-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3ECBA2F-F918-4B7F-9F2F-D7725B544921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D74532D-4199-438C-8152-221E01CBE36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16440" yWindow="7980" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ck_Old_Model" sheetId="1" r:id="rId1"/>
@@ -27,22 +27,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Ck _Obs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ck_old_model </t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Q_river</t>
+    <t>Qriver</t>
   </si>
   <si>
-    <t>Q_tide</t>
+    <t>Qtide</t>
   </si>
   <si>
-    <t>S_ocean</t>
+    <t>Socean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CkOldModel </t>
+  </si>
+  <si>
+    <t>CkObs</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:F1643"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -429,22 +429,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Updated lx experiment with new results
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Ck_Parameters_Estimation/0-Dataset/CK_OBS_WITH_FEATURES.xlsx
+++ b/Parameters-Estimation/Ck_Parameters_Estimation/0-Dataset/CK_OBS_WITH_FEATURES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\3_Estuarine Box Model\Experiments\Parameters-Estimation\Ck_Parameters_Estimation\0-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D74532D-4199-438C-8152-221E01CBE36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A275D4-FD19-414B-8AA6-2FD8D758578E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16440" yWindow="7980" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3945" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ck_Old_Model" sheetId="1" r:id="rId1"/>
@@ -413,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1643"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A1447" workbookViewId="0">
+      <selection activeCell="B1447" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>

</xml_diff>